<commit_message>
Added more skill tree text and readme.
</commit_message>
<xml_diff>
--- a/database/TECH_SKILLS.xlsx
+++ b/database/TECH_SKILLS.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/elijahkennard/Disinformation_Game/Operation_Otter/OperationOtter/database/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20E338DB-E3B9-854E-85CC-0A12222621A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E95536A-9160-4B4D-A1C6-0C2B3973577D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4340" yWindow="500" windowWidth="24460" windowHeight="15940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -332,7 +332,7 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>

</xml_diff>